<commit_message>
First start on pilot report
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,22 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Partners Project\Experiment 1 - Mimicry\Baseline Write-up\Cognition\R1\submitted\final submission\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25306"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9720"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25440" windowHeight="14240"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet1" sheetId="1" r:id="rId1"/>
     <sheet name="DataSet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -215,7 +213,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -250,7 +248,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -427,7 +425,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -438,12 +436,18 @@
   <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="7" max="7" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="11.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -490,7 +494,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -537,7 +541,7 @@
         <v>-0.81472</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15">
       <c r="A3">
         <v>1</v>
       </c>
@@ -584,7 +588,7 @@
         <v>-1.12137</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15">
       <c r="A4">
         <v>2</v>
       </c>
@@ -631,7 +635,7 @@
         <v>-0.29954999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="A5">
         <v>2</v>
       </c>
@@ -678,7 +682,7 @@
         <v>-0.81472</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15">
       <c r="A6">
         <v>3</v>
       </c>
@@ -725,7 +729,7 @@
         <v>0.31374999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15">
       <c r="A7">
         <v>3</v>
       </c>
@@ -772,7 +776,7 @@
         <v>-0.20141999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15">
       <c r="A8">
         <v>4</v>
       </c>
@@ -819,7 +823,7 @@
         <v>2.76694</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15">
       <c r="A9">
         <v>4</v>
       </c>
@@ -866,7 +870,7 @@
         <v>-0.29954999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15">
       <c r="A10">
         <v>6</v>
       </c>
@@ -913,7 +917,7 @@
         <v>0.51614000000000004</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15">
       <c r="A11">
         <v>6</v>
       </c>
@@ -960,7 +964,7 @@
         <v>-0.60619999999999996</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15">
       <c r="A12">
         <v>8</v>
       </c>
@@ -1007,7 +1011,7 @@
         <v>-0.20141999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15">
       <c r="A13">
         <v>8</v>
       </c>
@@ -1054,7 +1058,7 @@
         <v>-0.50807000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15">
       <c r="A14">
         <v>9</v>
       </c>
@@ -1101,7 +1105,7 @@
         <v>0.62039999999999995</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15">
       <c r="A15">
         <v>9</v>
       </c>
@@ -1148,7 +1152,7 @@
         <v>-1.2195</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15">
       <c r="A16">
         <v>10</v>
       </c>
@@ -1195,7 +1199,7 @@
         <v>2.1536499999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15">
       <c r="A17">
         <v>10</v>
       </c>
@@ -1242,7 +1246,7 @@
         <v>0.10523</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15">
       <c r="A18">
         <v>11</v>
       </c>
@@ -1289,7 +1293,7 @@
         <v>1.3318300000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15">
       <c r="A19">
         <v>11</v>
       </c>
@@ -1336,7 +1340,7 @@
         <v>-1.2195</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15">
       <c r="A20">
         <v>12</v>
       </c>
@@ -1383,7 +1387,7 @@
         <v>0.31374999999999997</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15">
       <c r="A21">
         <v>12</v>
       </c>
@@ -1430,7 +1434,7 @@
         <v>-0.91285000000000005</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15">
       <c r="A22">
         <v>13</v>
       </c>
@@ -1477,7 +1481,7 @@
         <v>1.6384799999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15">
       <c r="A23">
         <v>13</v>
       </c>
@@ -1524,7 +1528,7 @@
         <v>-0.29954999999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15">
       <c r="A24">
         <v>14</v>
       </c>
@@ -1571,7 +1575,7 @@
         <v>-9.7159999999999996E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15">
       <c r="A25">
         <v>14</v>
       </c>
@@ -1618,7 +1622,7 @@
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15">
       <c r="A26">
         <v>15</v>
       </c>
@@ -1665,7 +1669,7 @@
         <v>1.2337</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15">
       <c r="A27">
         <v>15</v>
       </c>
@@ -1712,7 +1716,7 @@
         <v>0.71853</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15">
       <c r="A28">
         <v>16</v>
       </c>
@@ -1759,7 +1763,7 @@
         <v>-0.29954999999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15">
       <c r="A29">
         <v>16</v>
       </c>
@@ -1806,7 +1810,7 @@
         <v>-0.50807000000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15">
       <c r="A30">
         <v>17</v>
       </c>
@@ -1853,7 +1857,7 @@
         <v>0.92705000000000004</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15">
       <c r="A31">
         <v>17</v>
       </c>
@@ -1900,7 +1904,7 @@
         <v>-1.12137</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15">
       <c r="A32">
         <v>18</v>
       </c>
@@ -1947,7 +1951,7 @@
         <v>0.71853</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15">
       <c r="A33">
         <v>18</v>
       </c>
@@ -1994,7 +1998,7 @@
         <v>0.10523</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15">
       <c r="A34">
         <v>19</v>
       </c>
@@ -2041,7 +2045,7 @@
         <v>-1.2195</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15">
       <c r="A35">
         <v>19</v>
       </c>
@@ -2088,7 +2092,7 @@
         <v>-1.32376</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15">
       <c r="A36">
         <v>20</v>
       </c>
@@ -2135,7 +2139,7 @@
         <v>0.31374999999999997</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15">
       <c r="A37">
         <v>20</v>
       </c>
@@ -2182,7 +2186,7 @@
         <v>-0.60619999999999996</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15">
       <c r="A38">
         <v>21</v>
       </c>
@@ -2229,7 +2233,7 @@
         <v>1.2337</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15">
       <c r="A39">
         <v>21</v>
       </c>
@@ -2278,6 +2282,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2289,9 +2298,16 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -2311,7 +2327,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>341.46</v>
       </c>
@@ -2331,7 +2347,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>286.43</v>
       </c>
@@ -2351,7 +2367,7 @@
         <v>21.08</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>215.27</v>
       </c>
@@ -2371,7 +2387,7 @@
         <v>29.15</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>305.86</v>
       </c>
@@ -2391,7 +2407,7 @@
         <v>20.79</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>416.4</v>
       </c>
@@ -2411,7 +2427,7 @@
         <v>56.19</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>365.07</v>
       </c>
@@ -2431,7 +2447,7 @@
         <v>17.46</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>451.6</v>
       </c>
@@ -2451,7 +2467,7 @@
         <v>34.270000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>291.2</v>
       </c>
@@ -2471,7 +2487,7 @@
         <v>14.42</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>348.93</v>
       </c>
@@ -2491,7 +2507,7 @@
         <v>65.92</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>390.2</v>
       </c>
@@ -2511,7 +2527,7 @@
         <v>83.17</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>570.88</v>
       </c>
@@ -2531,7 +2547,7 @@
         <v>6.38</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>281.31</v>
       </c>
@@ -2551,7 +2567,7 @@
         <v>28.95</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>413.77</v>
       </c>
@@ -2571,7 +2587,7 @@
         <v>1.57</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>269.60000000000002</v>
       </c>
@@ -2591,7 +2607,7 @@
         <v>91.53</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>653.62</v>
       </c>
@@ -2611,7 +2627,7 @@
         <v>36.68</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17">
         <v>497.69</v>
       </c>
@@ -2631,7 +2647,7 @@
         <v>159.74</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18">
         <v>298.5</v>
       </c>
@@ -2651,7 +2667,7 @@
         <v>7.25</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19">
         <v>298</v>
       </c>
@@ -2671,7 +2687,7 @@
         <v>11.7</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20">
         <v>502.5</v>
       </c>
@@ -2693,5 +2709,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>